<commit_message>
Update for board details functions were added to board manager and controller, also initializer for work with mongoDB for board collection only.
</commit_message>
<xml_diff>
--- a/Documents/Virtual Scrum Board Tasks.xlsx
+++ b/Documents/Virtual Scrum Board Tasks.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Fadi</t>
   </si>
@@ -210,12 +205,15 @@
   </si>
   <si>
     <t>Task should be updated with relevant comment changes</t>
+  </si>
+  <si>
+    <t>BoardView/BoardViewModel/BoardItemViewModel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,8 +249,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -307,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -359,7 +385,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -553,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -563,15 +589,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
@@ -713,7 +739,7 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>

</xml_diff>